<commit_message>
removing unwatned files and cleaning up code
</commit_message>
<xml_diff>
--- a/Data/Covariates/Temperature.xlsx
+++ b/Data/Covariates/Temperature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="2180" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="700" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sacramento_Drainage_Temperature" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -416,7 +416,7 @@
         <v>36464</v>
       </c>
       <c r="B1">
-        <v>44.4</v>
+        <v>46.8</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -425,7 +425,7 @@
         <v>36494</v>
       </c>
       <c r="B2">
-        <v>42.05</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -434,7 +434,7 @@
         <v>36525</v>
       </c>
       <c r="B3">
-        <v>40.65</v>
+        <v>43.5</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -443,7 +443,7 @@
         <v>36556</v>
       </c>
       <c r="B4">
-        <v>42.45</v>
+        <v>44.2</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -452,7 +452,7 @@
         <v>36585</v>
       </c>
       <c r="B5">
-        <v>54.5</v>
+        <v>56.9</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -461,7 +461,7 @@
         <v>36616</v>
       </c>
       <c r="B6">
-        <v>55.45</v>
+        <v>57.3</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -470,7 +470,7 @@
         <v>36646</v>
       </c>
       <c r="B7">
-        <v>60.5</v>
+        <v>63.2</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -479,7 +479,7 @@
         <v>36677</v>
       </c>
       <c r="B8">
-        <v>68.400000000000006</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -488,7 +488,7 @@
         <v>36707</v>
       </c>
       <c r="B9">
-        <v>74</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -497,7 +497,7 @@
         <v>36738</v>
       </c>
       <c r="B10">
-        <v>72.8</v>
+        <v>74.8</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -506,7 +506,7 @@
         <v>36769</v>
       </c>
       <c r="B11">
-        <v>67.25</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -515,7 +515,7 @@
         <v>36799</v>
       </c>
       <c r="B12">
-        <v>55.9</v>
+        <v>58.2</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -524,7 +524,7 @@
         <v>36830</v>
       </c>
       <c r="B13">
-        <v>45.7</v>
+        <v>47.7</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -533,7 +533,7 @@
         <v>36860</v>
       </c>
       <c r="B14">
-        <v>42.45</v>
+        <v>44.6</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -542,7 +542,7 @@
         <v>36891</v>
       </c>
       <c r="B15">
-        <v>41.25</v>
+        <v>44.1</v>
       </c>
       <c r="C15" s="1"/>
     </row>
@@ -551,7 +551,7 @@
         <v>36922</v>
       </c>
       <c r="B16">
-        <v>45.75</v>
+        <v>47.1</v>
       </c>
       <c r="C16" s="1"/>
     </row>
@@ -560,7 +560,7 @@
         <v>36950</v>
       </c>
       <c r="B17">
-        <v>49.1</v>
+        <v>51.1</v>
       </c>
       <c r="C17" s="1"/>
     </row>
@@ -569,7 +569,7 @@
         <v>36981</v>
       </c>
       <c r="B18">
-        <v>50.3</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1"/>
     </row>
@@ -578,7 +578,7 @@
         <v>37011</v>
       </c>
       <c r="B19">
-        <v>58.9</v>
+        <v>62.2</v>
       </c>
       <c r="C19" s="1"/>
     </row>
@@ -587,7 +587,7 @@
         <v>37042</v>
       </c>
       <c r="B20">
-        <v>63.1</v>
+        <v>66.3</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -596,7 +596,7 @@
         <v>37072</v>
       </c>
       <c r="B21">
-        <v>77</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="C21" s="1"/>
     </row>
@@ -605,7 +605,7 @@
         <v>37103</v>
       </c>
       <c r="B22">
-        <v>74.3</v>
+        <v>75.8</v>
       </c>
       <c r="C22" s="1"/>
     </row>
@@ -614,7 +614,7 @@
         <v>37134</v>
       </c>
       <c r="B23">
-        <v>64.400000000000006</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -623,7 +623,7 @@
         <v>37164</v>
       </c>
       <c r="B24">
-        <v>57.65</v>
+        <v>59.9</v>
       </c>
       <c r="C24" s="1"/>
     </row>
@@ -632,7 +632,7 @@
         <v>37195</v>
       </c>
       <c r="B25">
-        <v>50.05</v>
+        <v>46.1</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -641,7 +641,7 @@
         <v>37225</v>
       </c>
       <c r="B26">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -650,7 +650,7 @@
         <v>37256</v>
       </c>
       <c r="B27">
-        <v>42.1</v>
+        <v>44.6</v>
       </c>
       <c r="C27" s="1"/>
     </row>
@@ -659,7 +659,7 @@
         <v>37287</v>
       </c>
       <c r="B28">
-        <v>45.25</v>
+        <v>47.7</v>
       </c>
       <c r="C28" s="1"/>
     </row>
@@ -668,7 +668,7 @@
         <v>37315</v>
       </c>
       <c r="B29">
-        <v>40.9</v>
+        <v>44</v>
       </c>
       <c r="C29" s="1"/>
     </row>
@@ -677,7 +677,7 @@
         <v>37346</v>
       </c>
       <c r="B30">
-        <v>50.35</v>
+        <v>53</v>
       </c>
       <c r="C30" s="1"/>
     </row>
@@ -686,7 +686,7 @@
         <v>37376</v>
       </c>
       <c r="B31">
-        <v>62.2</v>
+        <v>64.599999999999994</v>
       </c>
       <c r="C31" s="1"/>
     </row>
@@ -695,7 +695,7 @@
         <v>37407</v>
       </c>
       <c r="B32">
-        <v>70.849999999999994</v>
+        <v>73.2</v>
       </c>
       <c r="C32" s="1"/>
     </row>
@@ -704,7 +704,7 @@
         <v>37437</v>
       </c>
       <c r="B33">
-        <v>77.349999999999994</v>
+        <v>79.3</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -713,7 +713,7 @@
         <v>37468</v>
       </c>
       <c r="B34">
-        <v>71.400000000000006</v>
+        <v>73.8</v>
       </c>
       <c r="C34" s="1"/>
     </row>
@@ -722,7 +722,7 @@
         <v>37499</v>
       </c>
       <c r="B35">
-        <v>67.599999999999994</v>
+        <v>69.5</v>
       </c>
       <c r="C35" s="1"/>
     </row>
@@ -731,7 +731,7 @@
         <v>37529</v>
       </c>
       <c r="B36">
-        <v>56.5</v>
+        <v>58.8</v>
       </c>
       <c r="C36" s="1"/>
     </row>
@@ -740,7 +740,7 @@
         <v>37560</v>
       </c>
       <c r="B37">
-        <v>47.85</v>
+        <v>51.3</v>
       </c>
       <c r="C37" s="1"/>
     </row>
@@ -749,7 +749,7 @@
         <v>37590</v>
       </c>
       <c r="B38">
-        <v>41.55</v>
+        <v>43.9</v>
       </c>
       <c r="C38" s="1"/>
     </row>
@@ -758,7 +758,7 @@
         <v>37621</v>
       </c>
       <c r="B39">
-        <v>39.5</v>
+        <v>41.5</v>
       </c>
       <c r="C39" s="1"/>
     </row>
@@ -767,7 +767,7 @@
         <v>37652</v>
       </c>
       <c r="B40">
-        <v>44.2</v>
+        <v>46.7</v>
       </c>
       <c r="C40" s="1"/>
     </row>
@@ -776,7 +776,7 @@
         <v>37680</v>
       </c>
       <c r="B41">
-        <v>52.25</v>
+        <v>54.5</v>
       </c>
       <c r="C41" s="1"/>
     </row>
@@ -785,7 +785,7 @@
         <v>37711</v>
       </c>
       <c r="B42">
-        <v>53.7</v>
+        <v>56.3</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -794,7 +794,7 @@
         <v>37741</v>
       </c>
       <c r="B43">
-        <v>62.05</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="C43" s="1"/>
     </row>
@@ -803,7 +803,7 @@
         <v>37772</v>
       </c>
       <c r="B44">
-        <v>68.3</v>
+        <v>70.5</v>
       </c>
       <c r="C44" s="1"/>
     </row>
@@ -812,7 +812,7 @@
         <v>37802</v>
       </c>
       <c r="B45">
-        <v>74.3</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="C45" s="1"/>
     </row>
@@ -821,7 +821,7 @@
         <v>37833</v>
       </c>
       <c r="B46">
-        <v>73.5</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="C46" s="1"/>
     </row>
@@ -830,7 +830,7 @@
         <v>37864</v>
       </c>
       <c r="B47">
-        <v>64.650000000000006</v>
+        <v>67.5</v>
       </c>
       <c r="C47" s="1"/>
     </row>
@@ -839,7 +839,7 @@
         <v>37894</v>
       </c>
       <c r="B48">
-        <v>55.55</v>
+        <v>58.6</v>
       </c>
       <c r="C48" s="1"/>
     </row>
@@ -848,7 +848,7 @@
         <v>37925</v>
       </c>
       <c r="B49">
-        <v>51</v>
+        <v>53.3</v>
       </c>
       <c r="C49" s="1"/>
     </row>
@@ -857,7 +857,7 @@
         <v>37955</v>
       </c>
       <c r="B50">
-        <v>39</v>
+        <v>41.2</v>
       </c>
       <c r="C50" s="1"/>
     </row>
@@ -866,7 +866,7 @@
         <v>37986</v>
       </c>
       <c r="B51">
-        <v>38.75</v>
+        <v>41.1</v>
       </c>
       <c r="C51" s="1"/>
     </row>
@@ -875,7 +875,7 @@
         <v>38017</v>
       </c>
       <c r="B52">
-        <v>43.45</v>
+        <v>45.8</v>
       </c>
       <c r="C52" s="1"/>
     </row>
@@ -884,7 +884,7 @@
         <v>38046</v>
       </c>
       <c r="B53">
-        <v>47.65</v>
+        <v>50.3</v>
       </c>
       <c r="C53" s="1"/>
     </row>
@@ -893,7 +893,7 @@
         <v>38077</v>
       </c>
       <c r="B54">
-        <v>51.5</v>
+        <v>54.4</v>
       </c>
       <c r="C54" s="1"/>
     </row>
@@ -902,7 +902,7 @@
         <v>38107</v>
       </c>
       <c r="B55">
-        <v>60.5</v>
+        <v>61.7</v>
       </c>
       <c r="C55" s="1"/>
     </row>
@@ -911,7 +911,7 @@
         <v>38138</v>
       </c>
       <c r="B56">
-        <v>68.75</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="C56" s="1"/>
     </row>
@@ -920,7 +920,7 @@
         <v>38168</v>
       </c>
       <c r="B57">
-        <v>74.599999999999994</v>
+        <v>76.5</v>
       </c>
       <c r="C57" s="1"/>
     </row>
@@ -929,7 +929,7 @@
         <v>38199</v>
       </c>
       <c r="B58">
-        <v>74.75</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="C58" s="1"/>
     </row>
@@ -938,7 +938,7 @@
         <v>38230</v>
       </c>
       <c r="B59">
-        <v>69.55</v>
+        <v>61.8</v>
       </c>
       <c r="C59" s="1"/>
     </row>
@@ -947,7 +947,7 @@
         <v>38260</v>
       </c>
       <c r="B60">
-        <v>59.45</v>
+        <v>57.8</v>
       </c>
       <c r="C60" s="1"/>
     </row>
@@ -956,7 +956,7 @@
         <v>38291</v>
       </c>
       <c r="B61">
-        <v>51.15</v>
+        <v>42</v>
       </c>
       <c r="C61" s="1"/>
     </row>
@@ -965,7 +965,7 @@
         <v>38321</v>
       </c>
       <c r="B62">
-        <v>39.35</v>
+        <v>37.9</v>
       </c>
       <c r="C62" s="1"/>
     </row>
@@ -974,7 +974,7 @@
         <v>38352</v>
       </c>
       <c r="B63">
-        <v>44.1</v>
+        <v>46.9</v>
       </c>
       <c r="C63" s="1"/>
     </row>
@@ -983,7 +983,7 @@
         <v>38383</v>
       </c>
       <c r="B64">
-        <v>43.15</v>
+        <v>45.3</v>
       </c>
       <c r="C64" s="1"/>
     </row>
@@ -992,7 +992,7 @@
         <v>38411</v>
       </c>
       <c r="B65">
-        <v>46.6</v>
+        <v>49.2</v>
       </c>
       <c r="C65" s="1"/>
     </row>
@@ -1001,7 +1001,7 @@
         <v>38442</v>
       </c>
       <c r="B66">
-        <v>52.1</v>
+        <v>54.3</v>
       </c>
       <c r="C66" s="1"/>
     </row>
@@ -1010,7 +1010,7 @@
         <v>38472</v>
       </c>
       <c r="B67">
-        <v>64.3</v>
+        <v>66.7</v>
       </c>
       <c r="C67" s="1"/>
     </row>
@@ -1019,7 +1019,7 @@
         <v>38503</v>
       </c>
       <c r="B68">
-        <v>65.7</v>
+        <v>67.5</v>
       </c>
       <c r="C68" s="1"/>
     </row>
@@ -1028,7 +1028,7 @@
         <v>38533</v>
       </c>
       <c r="B69">
-        <v>75.25</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="C69" s="1"/>
     </row>
@@ -1037,7 +1037,7 @@
         <v>38564</v>
       </c>
       <c r="B70">
-        <v>72.599999999999994</v>
+        <v>74.8</v>
       </c>
       <c r="C70" s="1"/>
     </row>
@@ -1046,7 +1046,7 @@
         <v>38595</v>
       </c>
       <c r="B71">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C71" s="1"/>
     </row>
@@ -1055,7 +1055,7 @@
         <v>38625</v>
       </c>
       <c r="B72">
-        <v>55.65</v>
+        <v>58.1</v>
       </c>
       <c r="C72" s="1"/>
     </row>
@@ -1064,7 +1064,7 @@
         <v>38656</v>
       </c>
       <c r="B73">
-        <v>48.2</v>
+        <v>41.8</v>
       </c>
       <c r="C73" s="1"/>
     </row>
@@ -1073,7 +1073,7 @@
         <v>38686</v>
       </c>
       <c r="B74">
-        <v>39.450000000000003</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="C74" s="1"/>
     </row>
@@ -1082,7 +1082,7 @@
         <v>38717</v>
       </c>
       <c r="B75">
-        <v>42.8</v>
+        <v>45.2</v>
       </c>
       <c r="C75" s="1"/>
     </row>
@@ -1091,7 +1091,7 @@
         <v>38748</v>
       </c>
       <c r="B76">
-        <v>44.7</v>
+        <v>46.8</v>
       </c>
       <c r="C76" s="1"/>
     </row>
@@ -1100,7 +1100,7 @@
         <v>38776</v>
       </c>
       <c r="B77">
-        <v>46.55</v>
+        <v>49</v>
       </c>
       <c r="C77" s="1"/>
     </row>
@@ -1109,7 +1109,7 @@
         <v>38807</v>
       </c>
       <c r="B78">
-        <v>47.9</v>
+        <v>50.9</v>
       </c>
       <c r="C78" s="1"/>
     </row>
@@ -1118,7 +1118,7 @@
         <v>38837</v>
       </c>
       <c r="B79">
-        <v>53.8</v>
+        <v>56.9</v>
       </c>
       <c r="C79" s="1"/>
     </row>
@@ -1127,7 +1127,7 @@
         <v>38868</v>
       </c>
       <c r="B80">
-        <v>66.849999999999994</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="C80" s="1"/>
     </row>
@@ -1136,7 +1136,7 @@
         <v>38898</v>
       </c>
       <c r="B81">
-        <v>74.05</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="C81" s="1"/>
     </row>
@@ -1145,7 +1145,7 @@
         <v>38929</v>
       </c>
       <c r="B82">
-        <v>72.5</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="C82" s="1"/>
     </row>
@@ -1154,7 +1154,7 @@
         <v>38960</v>
       </c>
       <c r="B83">
-        <v>69.5</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="C83" s="1"/>
     </row>
@@ -1163,7 +1163,7 @@
         <v>38990</v>
       </c>
       <c r="B84">
-        <v>58.7</v>
+        <v>60.5</v>
       </c>
       <c r="C84" s="1"/>
     </row>
@@ -1172,7 +1172,7 @@
         <v>39021</v>
       </c>
       <c r="B85">
-        <v>46.2</v>
+        <v>45.8</v>
       </c>
       <c r="C85" s="1"/>
     </row>
@@ -1181,7 +1181,7 @@
         <v>39051</v>
       </c>
       <c r="B86">
-        <v>43.1</v>
+        <v>41.1</v>
       </c>
       <c r="C86" s="1"/>
     </row>
@@ -1190,7 +1190,7 @@
         <v>39082</v>
       </c>
       <c r="B87">
-        <v>42.35</v>
+        <v>45.2</v>
       </c>
       <c r="C87" s="1"/>
     </row>
@@ -1199,7 +1199,7 @@
         <v>39113</v>
       </c>
       <c r="B88">
-        <v>41.4</v>
+        <v>43.5</v>
       </c>
       <c r="C88" s="1"/>
     </row>
@@ -1208,7 +1208,7 @@
         <v>39141</v>
       </c>
       <c r="B89">
-        <v>45.15</v>
+        <v>48.7</v>
       </c>
       <c r="C89" s="1"/>
     </row>
@@ -1217,7 +1217,7 @@
         <v>39172</v>
       </c>
       <c r="B90">
-        <v>50.2</v>
+        <v>53.4</v>
       </c>
       <c r="C90" s="1"/>
     </row>
@@ -1226,7 +1226,7 @@
         <v>39202</v>
       </c>
       <c r="B91">
-        <v>54.65</v>
+        <v>57.6</v>
       </c>
       <c r="C91" s="1"/>
     </row>
@@ -1235,7 +1235,7 @@
         <v>39233</v>
       </c>
       <c r="B92">
-        <v>64.05</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="C92" s="1"/>
     </row>
@@ -1244,7 +1244,7 @@
         <v>39263</v>
       </c>
       <c r="B93">
-        <v>71.849999999999994</v>
+        <v>74.2</v>
       </c>
       <c r="C93" s="1"/>
     </row>
@@ -1253,7 +1253,7 @@
         <v>39294</v>
       </c>
       <c r="B94">
-        <v>72.400000000000006</v>
+        <v>75.2</v>
       </c>
       <c r="C94" s="1"/>
     </row>
@@ -1262,7 +1262,7 @@
         <v>39325</v>
       </c>
       <c r="B95">
-        <v>70.849999999999994</v>
+        <v>72.3</v>
       </c>
       <c r="C95" s="1"/>
     </row>
@@ -1271,7 +1271,7 @@
         <v>39355</v>
       </c>
       <c r="B96">
-        <v>58.75</v>
+        <v>61.4</v>
       </c>
       <c r="C96" s="1"/>
     </row>
@@ -1280,7 +1280,7 @@
         <v>39386</v>
       </c>
       <c r="B97">
-        <v>46</v>
+        <v>42.8</v>
       </c>
       <c r="C97" s="1"/>
     </row>
@@ -1289,7 +1289,7 @@
         <v>39416</v>
       </c>
       <c r="B98">
-        <v>41.35</v>
+        <v>41</v>
       </c>
       <c r="C98" s="1"/>
     </row>
@@ -1298,7 +1298,7 @@
         <v>39447</v>
       </c>
       <c r="B99">
-        <v>44</v>
+        <v>46.5</v>
       </c>
       <c r="C99" s="1"/>
     </row>
@@ -1307,7 +1307,7 @@
         <v>39478</v>
       </c>
       <c r="B100">
-        <v>44.3</v>
+        <v>46.5</v>
       </c>
       <c r="C100" s="1"/>
     </row>
@@ -1316,7 +1316,7 @@
         <v>39507</v>
       </c>
       <c r="B101">
-        <v>45.8</v>
+        <v>48.8</v>
       </c>
       <c r="C101" s="1"/>
     </row>
@@ -1325,7 +1325,7 @@
         <v>39538</v>
       </c>
       <c r="B102">
-        <v>52.8</v>
+        <v>55.8</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -1334,7 +1334,7 @@
         <v>39568</v>
       </c>
       <c r="B103">
-        <v>61.2</v>
+        <v>63.9</v>
       </c>
       <c r="C103" s="1"/>
     </row>
@@ -1343,7 +1343,7 @@
         <v>39599</v>
       </c>
       <c r="B104">
-        <v>66.45</v>
+        <v>69.3</v>
       </c>
       <c r="C104" s="1"/>
     </row>
@@ -1352,7 +1352,7 @@
         <v>39629</v>
       </c>
       <c r="B105">
-        <v>72.7</v>
+        <v>74.7</v>
       </c>
       <c r="C105" s="1"/>
     </row>
@@ -1361,7 +1361,7 @@
         <v>39660</v>
       </c>
       <c r="B106">
-        <v>75.8</v>
+        <v>77.8</v>
       </c>
       <c r="C106" s="1"/>
     </row>
@@ -1370,7 +1370,7 @@
         <v>39691</v>
       </c>
       <c r="B107">
-        <v>71.150000000000006</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="C107" s="1"/>
     </row>
@@ -1379,7 +1379,7 @@
         <v>39721</v>
       </c>
       <c r="B108">
-        <v>59.55</v>
+        <v>62.2</v>
       </c>
       <c r="C108" s="1"/>
     </row>
@@ -1388,7 +1388,7 @@
         <v>39752</v>
       </c>
       <c r="B109">
-        <v>49.85</v>
+        <v>43</v>
       </c>
       <c r="C109" s="1"/>
     </row>
@@ -1397,7 +1397,7 @@
         <v>39782</v>
       </c>
       <c r="B110">
-        <v>40.299999999999997</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="C110" s="1"/>
     </row>
@@ -1406,7 +1406,7 @@
         <v>39813</v>
       </c>
       <c r="B111">
-        <v>39.85</v>
+        <v>42.1</v>
       </c>
       <c r="C111" s="1"/>
     </row>
@@ -1415,7 +1415,7 @@
         <v>39844</v>
       </c>
       <c r="B112">
-        <v>43.45</v>
+        <v>45.3</v>
       </c>
       <c r="C112" s="1"/>
     </row>
@@ -1424,7 +1424,7 @@
         <v>39872</v>
       </c>
       <c r="B113">
-        <v>51.05</v>
+        <v>53.8</v>
       </c>
       <c r="C113" s="1"/>
     </row>
@@ -1433,7 +1433,7 @@
         <v>39903</v>
       </c>
       <c r="B114">
-        <v>56.1</v>
+        <v>58.2</v>
       </c>
       <c r="C114" s="1"/>
     </row>
@@ -1442,7 +1442,7 @@
         <v>39933</v>
       </c>
       <c r="B115">
-        <v>61.45</v>
+        <v>63.8</v>
       </c>
       <c r="C115" s="1"/>
     </row>
@@ -1451,7 +1451,7 @@
         <v>39964</v>
       </c>
       <c r="B116">
-        <v>69.8</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="C116" s="1"/>
     </row>
@@ -1460,7 +1460,7 @@
         <v>39994</v>
       </c>
       <c r="B117">
-        <v>76.45</v>
+        <v>78</v>
       </c>
       <c r="C117" s="1"/>
     </row>
@@ -1469,7 +1469,7 @@
         <v>40025</v>
       </c>
       <c r="B118">
-        <v>72</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="C118" s="1"/>
     </row>
@@ -1478,7 +1478,7 @@
         <v>40056</v>
       </c>
       <c r="B119">
-        <v>66.5</v>
+        <v>69.3</v>
       </c>
       <c r="C119" s="1"/>
     </row>
@@ -1487,39 +1487,9 @@
         <v>40086</v>
       </c>
       <c r="B120">
-        <v>56.8</v>
+        <v>58.5</v>
       </c>
       <c r="C120" s="1"/>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="1"/>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="1"/>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="1"/>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="1"/>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="1"/>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" s="1"/>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="1"/>

</xml_diff>